<commit_message>
edit jacabian and update pic
</commit_message>
<xml_diff>
--- a/src/hw5/Acc_predict.xlsx
+++ b/src/hw5/Acc_predict.xlsx
@@ -385,1102 +385,1102 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>0.07197646168967266</v>
+        <v>0.07171025663944178</v>
       </c>
       <c r="B2">
-        <v>-0.1396017692485098</v>
+        <v>-0.1396787781993878</v>
       </c>
       <c r="C2">
-        <v>-9.79874128319476</v>
+        <v>-9.798742137540586</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>0.1500158285882179</v>
+        <v>0.1502230925831909</v>
       </c>
       <c r="B3">
-        <v>-0.3180924931204481</v>
+        <v>-0.3180632098250349</v>
       </c>
       <c r="C3">
-        <v>-9.793687375906657</v>
+        <v>-9.793685149983665</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>0.2275525360986123</v>
+        <v>0.2277698327481756</v>
       </c>
       <c r="B4">
-        <v>-0.4583486938032938</v>
+        <v>-0.4585568480562028</v>
       </c>
       <c r="C4">
-        <v>-9.786630488488054</v>
+        <v>-9.786615682675532</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>0.3088345611916764</v>
+        <v>0.2823941711250699</v>
       </c>
       <c r="B5">
-        <v>-0.609228499510386</v>
+        <v>-0.6360365387010967</v>
       </c>
       <c r="C5">
-        <v>-9.776168055490754</v>
+        <v>-9.77526015273004</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>0.3496735058184933</v>
+        <v>0.3723622926054082</v>
       </c>
       <c r="B6">
-        <v>-0.7872871238210684</v>
+        <v>-0.7780766707279367</v>
       </c>
       <c r="C6">
-        <v>-9.762064711114865</v>
+        <v>-9.761964096303295</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>0.4444639502270835</v>
+        <v>0.4336247806310334</v>
       </c>
       <c r="B7">
-        <v>-0.9288325982834721</v>
+        <v>-0.9487393847662435</v>
       </c>
       <c r="C7">
-        <v>-9.745754039647959</v>
+        <v>-9.744324662562105</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>0.4842872540977101</v>
+        <v>0.495718917547268</v>
       </c>
       <c r="B8">
-        <v>-1.109237539482687</v>
+        <v>-1.090334520276613</v>
       </c>
       <c r="C8">
-        <v>-9.724970845021639</v>
+        <v>-9.726532444231035</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>0.5693745632610725</v>
+        <v>0.577065441359715</v>
       </c>
       <c r="B9">
-        <v>-1.247330898263591</v>
+        <v>-1.259979679593396</v>
       </c>
       <c r="C9">
-        <v>-9.703606455176764</v>
+        <v>-9.701517751537645</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>0.6119311446011996</v>
+        <v>0.6269969257635979</v>
       </c>
       <c r="B10">
-        <v>-1.425383781928923</v>
+        <v>-1.41302875780626</v>
       </c>
       <c r="C10">
-        <v>-9.676457065914214</v>
+        <v>-9.677304613615069</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>0.6938470064130708</v>
+        <v>0.6952893760760148</v>
       </c>
       <c r="B11">
-        <v>-1.564963426937972</v>
+        <v>-1.576027874096695</v>
       </c>
       <c r="C11">
-        <v>-9.649324629425532</v>
+        <v>-9.647419801355495</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>0.7332887957991312</v>
+        <v>0.7459301912014321</v>
       </c>
       <c r="B12">
-        <v>-1.743212702082251</v>
+        <v>-1.734477423187499</v>
       </c>
       <c r="C12">
-        <v>-9.61579414386844</v>
+        <v>-9.616401417282196</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>0.8097934431710458</v>
+        <v>0.7895300975211763</v>
       </c>
       <c r="B13">
-        <v>-1.888063044249613</v>
+        <v>-1.892553935942289</v>
       </c>
       <c r="C13">
-        <v>-9.582246736561114</v>
+        <v>-9.583051801209132</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>0.8524931309288297</v>
+        <v>0.8589073972709946</v>
       </c>
       <c r="B14">
-        <v>-2.10020332833946</v>
+        <v>-2.059690927662287</v>
       </c>
       <c r="C14">
-        <v>-9.534275087354624</v>
+        <v>-9.54253380216276</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>0.9036176099622121</v>
+        <v>0.9008022774612778</v>
       </c>
       <c r="B15">
-        <v>-2.312055993381209</v>
+        <v>-2.207824400422208</v>
       </c>
       <c r="C15">
-        <v>-9.480394100375586</v>
+        <v>-9.50547561533987</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>0.9552838406484725</v>
+        <v>0.9714257701034302</v>
       </c>
       <c r="B16">
-        <v>-2.513579578438464</v>
+        <v>-2.361057422197073</v>
       </c>
       <c r="C16">
-        <v>-9.423871311019322</v>
+        <v>-9.461592879756932</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>0.9930432653212262</v>
+        <v>1.012580241986897</v>
       </c>
       <c r="B17">
-        <v>-2.721606845194245</v>
+        <v>-2.53688099579642</v>
       </c>
       <c r="C17">
-        <v>-9.361982762929655</v>
+        <v>-9.411637268122096</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>1.038103338625515</v>
+        <v>1.050823272175415</v>
       </c>
       <c r="B18">
-        <v>-2.95575325237739</v>
+        <v>-2.694357616075941</v>
       </c>
       <c r="C18">
-        <v>-9.285788290145058</v>
+        <v>-9.363557416246678</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>1.075491683088507</v>
+        <v>1.086441390589808</v>
       </c>
       <c r="B19">
-        <v>-3.160024963555391</v>
+        <v>-2.851073497817739</v>
       </c>
       <c r="C19">
-        <v>-9.21398718630074</v>
+        <v>-9.312949318817033</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>1.109063541090868</v>
+        <v>1.135769239164363</v>
       </c>
       <c r="B20">
-        <v>-3.374600327038969</v>
+        <v>-3.029411913492662</v>
       </c>
       <c r="C20">
-        <v>-9.133567249140473</v>
+        <v>-9.250550885961159</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>1.14249133934634</v>
+        <v>1.174913539566195</v>
       </c>
       <c r="B21">
-        <v>-3.572232532177795</v>
+        <v>-3.243845514687384</v>
       </c>
       <c r="C21">
-        <v>-9.053942140060826</v>
+        <v>-9.172624730761997</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>1.173576027128818</v>
+        <v>1.209455811068352</v>
       </c>
       <c r="B22">
-        <v>-3.76570242095289</v>
+        <v>-3.466705560999308</v>
       </c>
       <c r="C22">
-        <v>-8.971187467965326</v>
+        <v>-9.086207635444474</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>1.202037156919136</v>
+        <v>1.242198145230223</v>
       </c>
       <c r="B23">
-        <v>-3.956992318899224</v>
+        <v>-3.667277894567414</v>
       </c>
       <c r="C23">
-        <v>-8.884667605575252</v>
+        <v>-9.002667194337674</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>1.227760135330354</v>
+        <v>1.273819238807337</v>
       </c>
       <c r="B24">
-        <v>-4.14663529030379</v>
+        <v>-3.84766778163442</v>
       </c>
       <c r="C24">
-        <v>-8.794203819522311</v>
+        <v>-8.922602601764622</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>1.250703219704121</v>
+        <v>1.303885149841687</v>
       </c>
       <c r="B25">
-        <v>-4.3346515002789</v>
+        <v>-4.01700869295443</v>
       </c>
       <c r="C25">
-        <v>-8.699801022285031</v>
+        <v>-8.843275675718296</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>1.270861056113709</v>
+        <v>1.33131133261064</v>
       </c>
       <c r="B26">
-        <v>-4.520874141378566</v>
+        <v>-4.185192932843637</v>
       </c>
       <c r="C26">
-        <v>-8.601546905869212</v>
+        <v>-8.760808766919762</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>1.288249810753079</v>
+        <v>1.356482038334363</v>
       </c>
       <c r="B27">
-        <v>-4.705070210675758</v>
+        <v>-4.351417339917845</v>
       </c>
       <c r="C27">
-        <v>-8.499572150273581</v>
+        <v>-8.675547453246887</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>1.302900625589806</v>
+        <v>1.379341999951829</v>
       </c>
       <c r="B28">
-        <v>-4.886988303560911</v>
+        <v>-4.516028207355743</v>
       </c>
       <c r="C28">
-        <v>-8.394033314247482</v>
+        <v>-8.587368914722143</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>1.314856333351067</v>
+        <v>1.399876517334576</v>
       </c>
       <c r="B29">
-        <v>-5.066379012842051</v>
+        <v>-4.679002611310789</v>
       </c>
       <c r="C29">
-        <v>-8.285104496678374</v>
+        <v>-8.496309804824799</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>1.324169455701134</v>
+        <v>1.418083302422587</v>
       </c>
       <c r="B30">
-        <v>-5.243004431530622</v>
+        <v>-4.840234536404313</v>
       </c>
       <c r="C30">
-        <v>-8.172972518217495</v>
+        <v>-8.402450200982402</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>1.330900700926312</v>
+        <v>1.433965525927908</v>
       </c>
       <c r="B31">
-        <v>-5.416642994019106</v>
+        <v>-4.999600926913534</v>
       </c>
       <c r="C31">
-        <v>-8.057833579791632</v>
+        <v>-8.30588547007817</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>1.335117652812302</v>
+        <v>1.447529932398877</v>
       </c>
       <c r="B32">
-        <v>-5.587092111641988</v>
+        <v>-5.156978420933149</v>
       </c>
       <c r="C32">
-        <v>-7.939890590504181</v>
+        <v>-8.206718629320685</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>1.336893537337797</v>
+        <v>1.458786237990878</v>
       </c>
       <c r="B33">
-        <v>-5.754169615855174</v>
+        <v>-5.31224814188641</v>
       </c>
       <c r="C33">
-        <v>-7.819350849130223</v>
+        <v>-8.105057827731573</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>1.336306034802728</v>
+        <v>1.467746862203999</v>
       </c>
       <c r="B34">
-        <v>-5.917714454901217</v>
+        <v>-5.465297359226666</v>
       </c>
       <c r="C34">
-        <v>-7.696423962568786</v>
+        <v>-8.001015180820518</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>1.333436137850712</v>
+        <v>1.474426740627448</v>
       </c>
       <c r="B35">
-        <v>-6.077586861704076</v>
+        <v>-5.616020242688997</v>
       </c>
       <c r="C35">
-        <v>-7.571319964492043</v>
+        <v>-7.894705974273529</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>1.328367067594374</v>
+        <v>1.478843147968129</v>
       </c>
       <c r="B36">
-        <v>-6.233668117408861</v>
+        <v>-5.76431830705241</v>
       </c>
       <c r="C36">
-        <v>-7.444247627244207</v>
+        <v>-7.786247966683836</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>1.321183262352944</v>
+        <v>1.481015511476838</v>
       </c>
       <c r="B37">
-        <v>-6.385859995832611</v>
+        <v>-5.910100716516428</v>
       </c>
       <c r="C37">
-        <v>-7.315412968582374</v>
+        <v>-7.675760716397887</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>1.311969451631011</v>
+        <v>1.480965209976305</v>
       </c>
       <c r="B38">
-        <v>-6.534083956494667</v>
+        <v>-6.053284499031999</v>
       </c>
       <c r="C38">
-        <v>-7.185017954568104</v>
+        <v>-7.563364913887124</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>1.300809824412159</v>
+        <v>1.478715358466262</v>
       </c>
       <c r="B39">
-        <v>-6.678280144476162</v>
+        <v>-6.193794686627195</v>
       </c>
       <c r="C39">
-        <v>-7.053259396378974</v>
+        <v>-7.449181718050965</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>1.287787296856642</v>
+        <v>1.474290579881703</v>
       </c>
       <c r="B40">
-        <v>-6.818406248701324</v>
+        <v>-6.331564387819947</v>
       </c>
       <c r="C40">
-        <v>-6.920328034546155</v>
+        <v>-7.333332100004902</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>1.272982880705823</v>
+        <v>1.467716766132678</v>
       </c>
       <c r="B41">
-        <v>-6.95443626427768</v>
+        <v>-6.466534795602973</v>
       </c>
       <c r="C41">
-        <v>-6.786407800267343</v>
+        <v>-7.21593619925156</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>1.256475150412899</v>
+        <v>1.459020830721305</v>
       </c>
       <c r="B42">
-        <v>-7.086359198630623</v>
+        <v>-6.598655134143341</v>
       </c>
       <c r="C42">
-        <v>-6.651675240447183</v>
+        <v>-7.09711269715826</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>1.238339804363979</v>
+        <v>1.448230455235562</v>
       </c>
       <c r="B43">
-        <v>-7.214177755250224</v>
+        <v>-6.727882547662635</v>
       </c>
       <c r="C43">
-        <v>-6.51629909109309</v>
+        <v>-6.976978212190772</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>1.21864931355202</v>
+        <v>1.435373831940878</v>
       </c>
       <c r="B44">
-        <v>-7.337907023073486</v>
+        <v>-6.854181935423984</v>
       </c>
       <c r="C44">
-        <v>-6.380439982580201</v>
+        <v>-6.855646720673908</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>1.197472649700526</v>
+        <v>1.420479404564645</v>
       </c>
       <c r="B45">
-        <v>-7.457573194038105</v>
+        <v>-6.977525737164711</v>
       </c>
       <c r="C45">
-        <v>-6.24425025994182</v>
+        <v>-6.73322900608703</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>1.174875084078161</v>
+        <v>1.403575609215181</v>
       </c>
       <c r="B46">
-        <v>-7.573212326304414</v>
+        <v>-7.097893673612377</v>
       </c>
       <c r="C46">
-        <v>-6.107873901573543</v>
+        <v>-6.609832139117425</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>1.15091804803657</v>
+        <v>1.384690617209298</v>
       </c>
       <c r="B47">
-        <v>-7.684869166093844</v>
+        <v>-7.215272446886423</v>
       </c>
       <c r="C47">
-        <v>-5.971446520460836</v>
+        <v>-6.485558989926322</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>1.125659046469281</v>
+        <v>1.363852081413996</v>
       </c>
       <c r="B48">
-        <v>-7.792596037011934</v>
+        <v>-7.329655405614654</v>
       </c>
       <c r="C48">
-        <v>-5.835095433242523</v>
+        <v>-6.360507773359499</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>1.09915161563387</v>
+        <v>1.341086887548913</v>
       </c>
       <c r="B49">
-        <v>-7.89645180212659</v>
+        <v>-7.441042179489348</v>
       </c>
       <c r="C49">
-        <v>-5.698939784077492</v>
+        <v>-6.234771627181289</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>1.071445316823261</v>
+        <v>1.31642091175793</v>
       </c>
       <c r="B50">
-        <v>-7.996500901083187</v>
+        <v>-7.549438287762797</v>
       </c>
       <c r="C50">
-        <v>-5.563090712188083</v>
+        <v>-6.108438222847766</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>1.042585757151747</v>
+        <v>1.289878785651119</v>
       </c>
       <c r="B51">
-        <v>-8.092812462313171</v>
+        <v>-7.654854725849631</v>
       </c>
       <c r="C51">
-        <v>-5.427651553739699</v>
+        <v>-5.981589407880215</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>1.012614628442136</v>
+        <v>1.261483669951866</v>
       </c>
       <c r="B52">
-        <v>-8.185459488963037</v>
+        <v>-7.757307533778736</v>
       </c>
       <c r="C52">
-        <v>-5.292718070028853</v>
+        <v>-5.854300878569912</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>0.9815697551852711</v>
+        <v>1.231257037868119</v>
       </c>
       <c r="B53">
-        <v>-8.274518116360429</v>
+        <v>-7.856817349736182</v>
       </c>
       <c r="C53">
-        <v>-5.158378694680007</v>
+        <v>-5.726641881555434</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>0.9494851430019469</v>
+        <v>1.199218469350502</v>
       </c>
       <c r="B54">
-        <v>-8.360066938340456</v>
+        <v>-7.953408951378787</v>
       </c>
       <c r="C54">
-        <v>-5.024714792869882</v>
+        <v>-5.598674942778556</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>0.9163910199419707</v>
+        <v>1.165385457512331</v>
       </c>
       <c r="B55">
-        <v>-8.442186399300283</v>
+        <v>-8.047110786991478</v>
       </c>
       <c r="C55">
-        <v>-4.891800925838973</v>
+        <v>-5.470455622459996</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>0.8823138640716963</v>
+        <v>1.129773228676142</v>
       </c>
       <c r="B56">
-        <v>-8.520958248297351</v>
+        <v>-8.137954497927062</v>
       </c>
       <c r="C56">
-        <v>-4.759705114399443</v>
+        <v>-5.342032295057327</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>0.847276411821495</v>
+        <v>1.09239457778604</v>
       </c>
       <c r="B57">
-        <v>-8.596465050870057</v>
+        <v>-8.225974433120296</v>
       </c>
       <c r="C57">
-        <v>-4.62848909592975</v>
+        <v>-5.213445953692714</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>0.8112976422283142</v>
+        <v>1.053259721293002</v>
       </c>
       <c r="B58">
-        <v>-8.6687897536455</v>
+        <v>-8.311207155827617</v>
       </c>
       <c r="C58">
-        <v>-4.498208570398392</v>
+        <v>-5.084730039286416</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>0.7743927323685087</v>
+        <v>1.01237617008718</v>
       </c>
       <c r="B59">
-        <v>-8.738015296319546</v>
+        <v>-8.393690942127485</v>
       </c>
       <c r="C59">
-        <v>-4.368913432117932</v>
+        <v>-4.955910295625483</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>0.7365729788910387</v>
+        <v>0.9697486256220733</v>
       </c>
       <c r="B60">
-        <v>-8.80422426531824</v>
+        <v>-8.473465270147587</v>
       </c>
       <c r="C60">
-        <v>-4.240647985007607</v>
+        <v>-4.827004652857378</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>0.6978456796535073</v>
+        <v>0.9253789030513966</v>
       </c>
       <c r="B61">
-        <v>-8.86749858338074</v>
+        <v>-8.550570298489284</v>
       </c>
       <c r="C61">
-        <v>-4.113451139995407</v>
+        <v>-4.698023143448774</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>0.6582139680664829</v>
+        <v>0.8792658859769442</v>
       </c>
       <c r="B62">
-        <v>-8.927919229392998</v>
+        <v>-8.625046331930603</v>
       </c>
       <c r="C62">
-        <v>-3.987356593744397</v>
+        <v>-4.568967856508478</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>0.6176765908683848</v>
+        <v>0.8314055182734839</v>
       </c>
       <c r="B63">
-        <v>-8.985565982970522</v>
+        <v>-8.696933272247435</v>
       </c>
       <c r="C63">
-        <v>-3.862392988132648</v>
+        <v>-4.439832938552975</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>0.5762276176279237</v>
+        <v>0.7817908393924604</v>
       </c>
       <c r="B64">
-        <v>-9.040517188450078</v>
+        <v>-8.766270051949796</v>
       </c>
       <c r="C64">
-        <v>-3.738584049880595</v>
+        <v>-4.310604651290831</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>0.5338560671755914</v>
+        <v>0.7304120705118642</v>
       </c>
       <c r="B65">
-        <v>-9.092849533021209</v>
+        <v>-8.833094048950818</v>
       </c>
       <c r="C65">
-        <v>-3.615948709450368</v>
+        <v>-4.18126149979169</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>0.4905454321819924</v>
+        <v>0.6772567598356349</v>
       </c>
       <c r="B66">
-        <v>-9.142637833635867</v>
+        <v>-8.897440480747601</v>
       </c>
       <c r="C66">
-        <v>-3.494501197872946</v>
+        <v>-4.051774447425578</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>0.4462730779087605</v>
+        <v>0.6223099961644127</v>
       </c>
       <c r="B67">
-        <v>-9.189954827009128</v>
+        <v>-8.959341777687742</v>
       </c>
       <c r="C67">
-        <v>-3.374251119502739</v>
+        <v>-3.922107237092443</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>0.4010094842991521</v>
+        <v>0.5655547004360009</v>
       </c>
       <c r="B68">
-        <v>-9.234870956394905</v>
+        <v>-9.018826936425929</v>
       </c>
       <c r="C68">
-        <v>-3.255203497822527</v>
+        <v>-3.792216841322876</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>0.3547172914113039</v>
+        <v>0.506972005100109</v>
       </c>
       <c r="B69">
-        <v>-9.277454147799162</v>
+        <v>-9.075920856851674</v>
       </c>
       <c r="C69">
-        <v>-3.137358790233909</v>
+        <v>-3.662054066532822</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>0.3073500958241917</v>
+        <v>0.4465417307273571</v>
       </c>
       <c r="B70">
-        <v>-9.317769566759564</v>
+        <v>-9.130643668695081</v>
       </c>
       <c r="C70">
-        <v>-3.020712866090748</v>
+        <v>-3.53156433865185</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>0.2588509287858369</v>
+        <v>0.3842429678814452</v>
       </c>
       <c r="B71">
-        <v>-9.355879344599659</v>
+        <v>-9.183010057772904</v>
       </c>
       <c r="C71">
-        <v>-2.905256939749077</v>
+        <v>-3.400688697966248</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>0.2091503236871559</v>
+        <v>0.3200547696766083</v>
       </c>
       <c r="B72">
-        <v>-9.391842259901047</v>
+        <v>-9.233028606448665</v>
       </c>
       <c r="C72">
-        <v>-2.790977446565698</v>
+        <v>-3.26936502962088</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>0.1581638482817316</v>
+        <v>0.2539569562302859</v>
       </c>
       <c r="B73">
-        <v>-9.425713356443822</v>
+        <v>-9.280701168284359</v>
       </c>
       <c r="C73">
-        <v>-2.677855843628121</v>
+        <v>-3.137529551954468</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>0.1057889320689855</v>
+        <v>0.1859310260236635</v>
       </c>
       <c r="B74">
-        <v>-9.457543472473255</v>
+        <v>-9.326022302850735</v>
       </c>
       <c r="C74">
-        <v>-2.56586830685642</v>
+        <v>-3.005118576744099</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>0.05190075579669751</v>
+        <v>0.1159611606640216</v>
       </c>
       <c r="B75">
-        <v>-9.487378647001123</v>
+        <v>-9.368978802833297</v>
       </c>
       <c r="C75">
-        <v>-2.454985278973155</v>
+        <v>-2.872070542531616</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>-0.003653120039468938</v>
+        <v>0.04403529849454291</v>
       </c>
       <c r="B76">
-        <v>-9.515259355659964</v>
+        <v>-9.409549351261504</v>
       </c>
       <c r="C76">
-        <v>-2.345170793191729</v>
+        <v>-2.738328303666433</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>-0.06105983914128466</v>
+        <v>-0.0298537610406957</v>
       </c>
       <c r="B77">
-        <v>-9.54121950947089</v>
+        <v>-9.447704350943106</v>
       </c>
       <c r="C77">
-        <v>-2.236381445133212</v>
+        <v>-2.603841633072649</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>-0.1205506796973066</v>
+        <v>-0.1057072759548745</v>
       </c>
       <c r="B78">
-        <v>-9.565285121904985</v>
+        <v>-9.483405969753154</v>
       </c>
       <c r="C78">
-        <v>-2.128564791188574</v>
+        <v>-2.468569866270841</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>-0.1824137209773076</v>
+        <v>-0.1835195734922435</v>
       </c>
       <c r="B79">
-        <v>-9.587472508700113</v>
+        <v>-9.516608442832874</v>
       </c>
       <c r="C79">
-        <v>-2.021656778317914</v>
+        <v>-2.332484579144587</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>-0.2470109822181712</v>
+        <v>-0.263277241283689</v>
       </c>
       <c r="B80">
-        <v>-9.607785825607486</v>
+        <v>-9.547258664470432</v>
       </c>
       <c r="C80">
-        <v>-1.915577485751879</v>
+        <v>-2.195572155023907</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>-0.3148016913769558</v>
+        <v>-0.3449585965446406</v>
       </c>
       <c r="B81">
-        <v>-9.626213666325132</v>
+        <v>-9.575297087187284</v>
       </c>
       <c r="C81">
-        <v>-1.810223838469001</v>
+        <v>-2.057836062171295</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>-0.3863736949616374</v>
+        <v>-0.4285335375762744</v>
       </c>
       <c r="B82">
-        <v>-9.642724339449366</v>
+        <v>-9.600658922735068</v>
       </c>
       <c r="C82">
-        <v>-1.705456736839862</v>
+        <v>-1.919298636606591</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>-0.4624846933571209</v>
+        <v>-0.5139638763192418</v>
       </c>
       <c r="B83">
-        <v>-9.657259366266619</v>
+        <v>-9.623275609890943</v>
       </c>
       <c r="C83">
-        <v>-1.601077587459789</v>
+        <v>-1.780002154469767</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>-0.544111711163165</v>
+        <v>-0.6012042295619848</v>
       </c>
       <c r="B84">
-        <v>-9.669724924716663</v>
+        <v>-9.643076479352121</v>
       </c>
       <c r="C84">
-        <v>-1.496783994465623</v>
+        <v>-1.640008990134715</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>-0.6324928779197341</v>
+        <v>-0.6902035053985314</v>
       </c>
       <c r="B85">
-        <v>-9.67998238552391</v>
+        <v>-9.659990510871214</v>
       </c>
       <c r="C85">
-        <v>-1.392082531794596</v>
+        <v>-1.499400697283322</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>-0.7290919209015976</v>
+        <v>-0.7809069573808535</v>
       </c>
       <c r="B86">
-        <v>-9.687845426205932</v>
+        <v>-9.673948048200453</v>
       </c>
       <c r="C86">
-        <v>-1.28610884796615</v>
+        <v>-1.358275923600515</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>-0.8352317188292702</v>
+        <v>-0.8732586892876641</v>
       </c>
       <c r="B87">
-        <v>-9.693114592672789</v>
+        <v>-9.684882321157531</v>
       </c>
       <c r="C87">
-        <v>-1.177249960363288</v>
+        <v>-1.21674717460693</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>-0.9505870560672358</v>
+        <v>-0.9672043739548937</v>
       </c>
       <c r="B88">
-        <v>-9.695753230897735</v>
+        <v>-9.692730630230306</v>
       </c>
       <c r="C88">
-        <v>-1.062428131392224</v>
+        <v>-1.07493656966247</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>-1.061472031401462</v>
+        <v>-1.056089880039871</v>
       </c>
       <c r="B89">
-        <v>-9.698004131564327</v>
+        <v>-9.697142000411628</v>
       </c>
       <c r="C89">
-        <v>-0.9284357762999722</v>
+        <v>-0.9434570414863348</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>-1.159502481008963</v>
+        <v>-1.164371591367519</v>
       </c>
       <c r="B90">
-        <v>-9.698492321900074</v>
+        <v>-9.699837340056414</v>
       </c>
       <c r="C90">
-        <v>-0.7967437973272196</v>
+        <v>-0.7729129146699805</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>-1.254420142659921</v>
+        <v>-1.266053242519829</v>
       </c>
       <c r="B91">
-        <v>-9.697621389041899</v>
+        <v>-9.696427202481912</v>
       </c>
       <c r="C91">
-        <v>-0.650053459713984</v>
+        <v>-0.6452973687175767</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>-1.352676884048848</v>
+        <v>-1.36015216921549</v>
       </c>
       <c r="B92">
-        <v>-9.692684865046999</v>
+        <v>-9.692050206003014</v>
       </c>
       <c r="C92">
-        <v>-0.5119817909347537</v>
+        <v>-0.5041318090493085</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>-1.44771402739686</v>
+        <v>-1.449985390296962</v>
       </c>
       <c r="B93">
-        <v>-9.685761377223525</v>
+        <v>-9.685317640315198</v>
       </c>
       <c r="C93">
-        <v>-0.3607639648903556</v>
+        <v>-0.3635444596258592</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>-1.546026660095558</v>
+        <v>-1.55036103661426</v>
       </c>
       <c r="B94">
-        <v>-9.674822927349524</v>
+        <v>-9.674013049355789</v>
       </c>
       <c r="C94">
-        <v>-0.218180866956228</v>
+        <v>-0.2232760108973482</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>-1.646607168787393</v>
+        <v>-1.652542135016201</v>
       </c>
       <c r="B95">
-        <v>-9.660340476750967</v>
+        <v>-9.659300236368669</v>
       </c>
       <c r="C95">
-        <v>-0.08066414906805441</v>
+        <v>-0.08380594062642555</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>-1.750528114700273</v>
+        <v>-1.756757181048228</v>
       </c>
       <c r="B96">
-        <v>-9.642265417926261</v>
+        <v>-9.641098592656835</v>
       </c>
       <c r="C96">
-        <v>0.04867165404224494</v>
+        <v>0.05497393478664492</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>-1.853360148768037</v>
+        <v>-1.863260231586666</v>
       </c>
       <c r="B97">
-        <v>-9.62141116599094</v>
+        <v>-9.619300030991074</v>
       </c>
       <c r="C97">
-        <v>0.1830391594806411</v>
+        <v>0.1932051323405597</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>-1.957786729636462</v>
+        <v>-1.972319448066795</v>
       </c>
       <c r="B98">
-        <v>-9.597214406901115</v>
+        <v>-9.593766624196313</v>
       </c>
       <c r="C98">
-        <v>0.3170910740293076</v>
+        <v>0.3310558189103592</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>-2.054744718610656</v>
+        <v>-2.084199422059882</v>
       </c>
       <c r="B99">
-        <v>-9.570751962127279</v>
+        <v>-9.564330778817173</v>
       </c>
       <c r="C99">
-        <v>0.4676868832653795</v>
+        <v>0.4687104889543257</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>-2.160274169760205</v>
+        <v>-2.199134790291331</v>
       </c>
       <c r="B100">
-        <v>-9.540242608635923</v>
+        <v>-9.530799554268567</v>
       </c>
       <c r="C100">
-        <v>0.5974834556994066</v>
+        <v>0.6063547068213584</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>-2.265119402272404</v>
+        <v>-2.31729150682945</v>
       </c>
       <c r="B101">
-        <v>-9.506652526626816</v>
+        <v>-9.492965624734099</v>
       </c>
       <c r="C101">
-        <v>0.7299259081777114</v>
+        <v>0.7441530218932497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>